<commit_message>
upgrade node version to 18
</commit_message>
<xml_diff>
--- a/cypress/e2e/Reports/BalanceChecker/Settlement_Balance.xlsx
+++ b/cypress/e2e/Reports/BalanceChecker/Settlement_Balance.xlsx
@@ -442,7 +442,7 @@
         <v>2025/01/25</v>
       </c>
       <c r="B2" t="str">
-        <v>2025/01/31</v>
+        <v>2025/02/03</v>
       </c>
       <c r="C2" t="str">
         <v>AC2374426306</v>
@@ -454,10 +454,10 @@
         <v>2520293169</v>
       </c>
       <c r="F2" t="str">
-        <v>4,937,185.00</v>
+        <v>6,643,197.00</v>
       </c>
       <c r="G2" t="str">
-        <v>4,838,441.30</v>
+        <v>6,510,333.06</v>
       </c>
       <c r="H2" t="str">
         <v>pending</v>
@@ -477,7 +477,7 @@
         <v>2025/01/25</v>
       </c>
       <c r="B3" t="str">
-        <v>2025/01/31</v>
+        <v>2025/02/03</v>
       </c>
       <c r="C3" t="str">
         <v>AC2473062452</v>
@@ -489,10 +489,10 @@
         <v>2551923888</v>
       </c>
       <c r="F3" t="str">
-        <v>1,688,761.00</v>
+        <v>2,973,505.00</v>
       </c>
       <c r="G3" t="str">
-        <v>1,641,020.37</v>
+        <v>2,889,765.51</v>
       </c>
       <c r="H3" t="str">
         <v>pending</v>
@@ -512,7 +512,7 @@
         <v>2025/01/25</v>
       </c>
       <c r="B4" t="str">
-        <v>2025/01/31</v>
+        <v>2025/02/03</v>
       </c>
       <c r="C4" t="str">
         <v>AC2347670819</v>
@@ -524,10 +524,10 @@
         <v>2594791110</v>
       </c>
       <c r="F4" t="str">
-        <v>289,116.00</v>
+        <v>322,416.00</v>
       </c>
       <c r="G4" t="str">
-        <v>277,383.36</v>
+        <v>309,308.36</v>
       </c>
       <c r="H4" t="str">
         <v>pending</v>
@@ -547,7 +547,7 @@
         <v>2025/01/11</v>
       </c>
       <c r="B5" t="str">
-        <v>2025/01/31</v>
+        <v>2025/02/03</v>
       </c>
       <c r="C5" t="str">
         <v>AC2346446835</v>
@@ -559,10 +559,10 @@
         <v>2445605593</v>
       </c>
       <c r="F5" t="str">
-        <v>2,492.00</v>
+        <v>10,267.00</v>
       </c>
       <c r="G5" t="str">
-        <v>2,267.00</v>
+        <v>9,717.00</v>
       </c>
       <c r="H5" t="str">
         <v>pending</v>
@@ -582,7 +582,7 @@
         <v>2024/11/16</v>
       </c>
       <c r="B6" t="str">
-        <v>2025/01/31</v>
+        <v>2025/02/03</v>
       </c>
       <c r="C6" t="str">
         <v>AC2313592098</v>
@@ -594,10 +594,10 @@
         <v>2448243172</v>
       </c>
       <c r="F6" t="str">
-        <v>919,153.00</v>
+        <v>929,085.00</v>
       </c>
       <c r="G6" t="str">
-        <v>900,769.94</v>
+        <v>910,503.30</v>
       </c>
       <c r="H6" t="str">
         <v>pending</v>

</xml_diff>

<commit_message>
resolve checkout branch conflict
</commit_message>
<xml_diff>
--- a/cypress/e2e/Reports/BalanceChecker/Settlement_Balance.xlsx
+++ b/cypress/e2e/Reports/BalanceChecker/Settlement_Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workplace\PAYSTAGE-AUTOMATION\cypress\e2e\Reports\BalanceChecker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3561A2-6DEA-4287-AC9B-BB01643A51C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202829E2-017C-4FD2-9264-4A2CC2224853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SETTLEMENT BALANCE" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:K965"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>